<commit_message>
Update microstate and microstate pair lists by adding SM21_micro020.
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM21_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM21_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Microstate List</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>c1cc(cc(c1)Br)Nc2c(c[nH]c(=Nc3cccc(c3)Br)n2)F</t>
+  </si>
+  <si>
+    <t>SM21_micro020</t>
+  </si>
+  <si>
+    <t>c1cc(cc(c1)Br)Nc2c(cnc(n2)Nc3cccc(c3)Br)F</t>
   </si>
   <si>
     <t>SM21_micro021</t>
@@ -1208,6 +1214,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="73332975"/>
+          <a:ext cx="3175163" cy="3175163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3175163</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="tmp26.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="76504800"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1505,7 +1549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1676,37 +1720,37 @@
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>45</v>
@@ -1798,6 +1842,17 @@
       </c>
       <c r="D26" s="3" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" s="2" customFormat="1" ht="250.0" customHeight="1">
+      <c r="B27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>